<commit_message>
[ADDED] optional conversion of date columns and according tests
</commit_message>
<xml_diff>
--- a/tests/INPUT/example_001.xlsx
+++ b/tests/INPUT/example_001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="master_table" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="301">
   <si>
     <t xml:space="preserve">TID</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">pH</t>
   </si>
   <si>
+    <t xml:space="preserve">sequencing date</t>
+  </si>
+  <si>
     <t xml:space="preserve">NA</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
     <t xml:space="preserve">TRUE</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-04</t>
+  </si>
+  <si>
     <t xml:space="preserve">T10</t>
   </si>
   <si>
@@ -88,6 +94,9 @@
     <t xml:space="preserve">FALSE</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-18</t>
+  </si>
+  <si>
     <t xml:space="preserve">T11</t>
   </si>
   <si>
@@ -100,6 +109,9 @@
     <t xml:space="preserve">Asia</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-25</t>
+  </si>
+  <si>
     <t xml:space="preserve">T12</t>
   </si>
   <si>
@@ -109,6 +121,9 @@
     <t xml:space="preserve">B. subtilis 1099</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-15</t>
+  </si>
+  <si>
     <t xml:space="preserve">T13</t>
   </si>
   <si>
@@ -121,6 +136,9 @@
     <t xml:space="preserve">Europe</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-01</t>
+  </si>
+  <si>
     <t xml:space="preserve">T14</t>
   </si>
   <si>
@@ -130,6 +148,9 @@
     <t xml:space="preserve">B. subtilis 1153</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-07</t>
+  </si>
+  <si>
     <t xml:space="preserve">T15</t>
   </si>
   <si>
@@ -139,6 +160,9 @@
     <t xml:space="preserve">B. subtilis 117</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-11</t>
+  </si>
+  <si>
     <t xml:space="preserve">T16</t>
   </si>
   <si>
@@ -148,6 +172,9 @@
     <t xml:space="preserve">B. subtilis 118</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-03</t>
+  </si>
+  <si>
     <t xml:space="preserve">T17</t>
   </si>
   <si>
@@ -175,12 +202,18 @@
     <t xml:space="preserve">B. subtilis 124</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-NN</t>
+  </si>
+  <si>
     <t xml:space="preserve">Basu56</t>
   </si>
   <si>
     <t xml:space="preserve">B. subtilis 56</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-08</t>
+  </si>
+  <si>
     <t xml:space="preserve">T20</t>
   </si>
   <si>
@@ -190,6 +223,9 @@
     <t xml:space="preserve">B. subtilis 128</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-17</t>
+  </si>
+  <si>
     <t xml:space="preserve">T21</t>
   </si>
   <si>
@@ -211,6 +247,9 @@
     <t xml:space="preserve">B. subtilis 1335</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-03</t>
+  </si>
+  <si>
     <t xml:space="preserve">T23</t>
   </si>
   <si>
@@ -220,6 +259,9 @@
     <t xml:space="preserve">B. subtilis 134</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-02</t>
+  </si>
+  <si>
     <t xml:space="preserve">T24</t>
   </si>
   <si>
@@ -238,6 +280,9 @@
     <t xml:space="preserve">B. subtilis 1389</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-10</t>
+  </si>
+  <si>
     <t xml:space="preserve">T26</t>
   </si>
   <si>
@@ -247,6 +292,9 @@
     <t xml:space="preserve">B. subtilis 145</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-18</t>
+  </si>
+  <si>
     <t xml:space="preserve">T27</t>
   </si>
   <si>
@@ -256,6 +304,9 @@
     <t xml:space="preserve">B. subtilis 1504</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-15</t>
+  </si>
+  <si>
     <t xml:space="preserve">T28</t>
   </si>
   <si>
@@ -283,6 +334,9 @@
     <t xml:space="preserve">Gen. sp. NKA14365</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-20</t>
+  </si>
+  <si>
     <t xml:space="preserve">T30</t>
   </si>
   <si>
@@ -301,6 +355,9 @@
     <t xml:space="preserve">B. subtilis 176</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-16</t>
+  </si>
+  <si>
     <t xml:space="preserve">T32</t>
   </si>
   <si>
@@ -310,6 +367,9 @@
     <t xml:space="preserve">B. subtilis 1828</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-09</t>
+  </si>
+  <si>
     <t xml:space="preserve">T33</t>
   </si>
   <si>
@@ -319,6 +379,9 @@
     <t xml:space="preserve">B. subtilis 185</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-22</t>
+  </si>
+  <si>
     <t xml:space="preserve">T34</t>
   </si>
   <si>
@@ -328,6 +391,9 @@
     <t xml:space="preserve">B. subtilis 1866</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-30</t>
+  </si>
+  <si>
     <t xml:space="preserve">Basu1871</t>
   </si>
   <si>
@@ -343,6 +409,9 @@
     <t xml:space="preserve">B. subtilis 204</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-23</t>
+  </si>
+  <si>
     <t xml:space="preserve">T37</t>
   </si>
   <si>
@@ -388,6 +457,9 @@
     <t xml:space="preserve">B. subtilis 260</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-24</t>
+  </si>
+  <si>
     <t xml:space="preserve">T41</t>
   </si>
   <si>
@@ -442,6 +514,9 @@
     <t xml:space="preserve">B. subtilis 302</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-01</t>
+  </si>
+  <si>
     <t xml:space="preserve">T47</t>
   </si>
   <si>
@@ -469,6 +544,9 @@
     <t xml:space="preserve">B. subtilis 321</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-05</t>
+  </si>
+  <si>
     <t xml:space="preserve">T5</t>
   </si>
   <si>
@@ -478,6 +556,9 @@
     <t xml:space="preserve">B. subtilis 1000</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-02-28</t>
+  </si>
+  <si>
     <t xml:space="preserve">T50</t>
   </si>
   <si>
@@ -487,6 +568,9 @@
     <t xml:space="preserve">B. subtilis 326</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-02-27</t>
+  </si>
+  <si>
     <t xml:space="preserve">T51</t>
   </si>
   <si>
@@ -577,6 +661,9 @@
     <t xml:space="preserve">B. subtilis 1008</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-11</t>
+  </si>
+  <si>
     <t xml:space="preserve">T60</t>
   </si>
   <si>
@@ -586,6 +673,9 @@
     <t xml:space="preserve">B. subtilis 388</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-02-29</t>
+  </si>
+  <si>
     <t xml:space="preserve">T61</t>
   </si>
   <si>
@@ -604,6 +694,9 @@
     <t xml:space="preserve">B. subtilis 406</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-08</t>
+  </si>
+  <si>
     <t xml:space="preserve">T63</t>
   </si>
   <si>
@@ -661,6 +754,9 @@
     <t xml:space="preserve">B. subtilis 542</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-09</t>
+  </si>
+  <si>
     <t xml:space="preserve">T69</t>
   </si>
   <si>
@@ -670,6 +766,9 @@
     <t xml:space="preserve">B. subtilis 590</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-07</t>
+  </si>
+  <si>
     <t xml:space="preserve">T7</t>
   </si>
   <si>
@@ -679,6 +778,9 @@
     <t xml:space="preserve">B. subtilis 1014</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-13</t>
+  </si>
+  <si>
     <t xml:space="preserve">T70</t>
   </si>
   <si>
@@ -697,6 +799,9 @@
     <t xml:space="preserve">B. subtilis 693</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-14</t>
+  </si>
+  <si>
     <t xml:space="preserve">T72</t>
   </si>
   <si>
@@ -706,6 +811,9 @@
     <t xml:space="preserve">B. subtilis 726</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-02</t>
+  </si>
+  <si>
     <t xml:space="preserve">T73</t>
   </si>
   <si>
@@ -760,6 +868,9 @@
     <t xml:space="preserve">B. subtilis 1128</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-20</t>
+  </si>
+  <si>
     <t xml:space="preserve">T79</t>
   </si>
   <si>
@@ -769,6 +880,9 @@
     <t xml:space="preserve">B. subtilis 26</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-03-27</t>
+  </si>
+  <si>
     <t xml:space="preserve">T8</t>
   </si>
   <si>
@@ -796,6 +910,9 @@
     <t xml:space="preserve">B. subtilis GT47</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-04-06</t>
+  </si>
+  <si>
     <t xml:space="preserve">T9</t>
   </si>
   <si>
@@ -803,15 +920,19 @@
   </si>
   <si>
     <t xml:space="preserve">B. subtilis 1036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-12-NN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -899,7 +1020,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -922,6 +1043,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1001,16 +1130,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L82"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1:M82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1022" min="1" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1" style="1" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,28 +1179,31 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0</v>
@@ -1088,28 +1220,31 @@
       <c r="L2" s="5" t="n">
         <v>9.059291</v>
       </c>
+      <c r="M2" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>1991</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>9</v>
@@ -1126,28 +1261,31 @@
       <c r="L3" s="5" t="n">
         <v>3.993843</v>
       </c>
+      <c r="M3" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1994</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>12</v>
@@ -1164,28 +1302,31 @@
       <c r="L4" s="5" t="n">
         <v>2.871438</v>
       </c>
+      <c r="M4" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>1991</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>1</v>
@@ -1202,28 +1343,31 @@
       <c r="L5" s="5" t="n">
         <v>10.41766</v>
       </c>
+      <c r="M5" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>1994</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>13</v>
@@ -1240,28 +1384,31 @@
       <c r="L6" s="5" t="n">
         <v>12.96324</v>
       </c>
+      <c r="M6" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>1994</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>17</v>
@@ -1278,28 +1425,31 @@
       <c r="L7" s="5" t="n">
         <v>12.38771</v>
       </c>
+      <c r="M7" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>1985</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>24</v>
@@ -1316,28 +1466,31 @@
       <c r="L8" s="5" t="n">
         <v>10.87573</v>
       </c>
+      <c r="M8" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>1985</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>10</v>
@@ -1354,28 +1507,31 @@
       <c r="L9" s="5" t="n">
         <v>7.08382</v>
       </c>
+      <c r="M9" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>1991</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>13</v>
@@ -1392,28 +1548,31 @@
       <c r="L10" s="5" t="n">
         <v>8.463543</v>
       </c>
+      <c r="M10" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>1981</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>18</v>
@@ -1430,28 +1589,31 @@
       <c r="L11" s="5" t="n">
         <v>6.003661</v>
       </c>
+      <c r="M11" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>1980</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>22</v>
@@ -1468,28 +1630,31 @@
       <c r="L12" s="5" t="n">
         <v>12.17484</v>
       </c>
+      <c r="M12" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F13" s="1" t="n">
         <v>1980</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>24</v>
@@ -1506,28 +1671,31 @@
       <c r="L13" s="5" t="n">
         <v>2.48023</v>
       </c>
+      <c r="M13" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>1981</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>24</v>
@@ -1544,28 +1712,31 @@
       <c r="L14" s="5" t="n">
         <v>12.71314</v>
       </c>
+      <c r="M14" s="6" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>1983</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>2</v>
@@ -1582,28 +1753,31 @@
       <c r="L15" s="5" t="n">
         <v>12.54398</v>
       </c>
+      <c r="M15" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F16" s="1" t="n">
         <v>1995</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>3</v>
@@ -1620,28 +1794,31 @@
       <c r="L16" s="5" t="n">
         <v>10.47492</v>
       </c>
+      <c r="M16" s="6" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>1980</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>4</v>
@@ -1658,28 +1835,31 @@
       <c r="L17" s="5" t="n">
         <v>2.864752</v>
       </c>
+      <c r="M17" s="6" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>1984</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>11</v>
@@ -1696,28 +1876,31 @@
       <c r="L18" s="5" t="n">
         <v>4.858033</v>
       </c>
+      <c r="M18" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>1996</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>5</v>
@@ -1734,28 +1917,31 @@
       <c r="L19" s="5" t="n">
         <v>4.541709</v>
       </c>
+      <c r="M19" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>1983</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>24</v>
@@ -1772,28 +1958,31 @@
       <c r="L20" s="5" t="n">
         <v>7.364183</v>
       </c>
+      <c r="M20" s="6" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F21" s="1" t="n">
         <v>1996</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H21" s="1" t="n">
         <v>24</v>
@@ -1810,28 +1999,31 @@
       <c r="L21" s="5" t="n">
         <v>12.51478</v>
       </c>
+      <c r="M21" s="6" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>1997</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>24</v>
@@ -1848,28 +2040,31 @@
       <c r="L22" s="5" t="n">
         <v>3.15453</v>
       </c>
+      <c r="M22" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>1998</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>6</v>
@@ -1886,28 +2081,31 @@
       <c r="L23" s="5" t="n">
         <v>11.85583</v>
       </c>
+      <c r="M23" s="6" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>7</v>
@@ -1924,28 +2122,31 @@
       <c r="L24" s="5" t="n">
         <v>4.02289</v>
       </c>
+      <c r="M24" s="6" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F25" s="1" t="n">
         <v>1999</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H25" s="1" t="n">
         <v>10</v>
@@ -1962,28 +2163,31 @@
       <c r="L25" s="5" t="n">
         <v>4.837152</v>
       </c>
+      <c r="M25" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F26" s="1" t="n">
         <v>1986</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>21</v>
@@ -2000,28 +2204,31 @@
       <c r="L26" s="5" t="n">
         <v>10.82208</v>
       </c>
+      <c r="M26" s="6" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>2000</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>25</v>
@@ -2038,28 +2245,31 @@
       <c r="L27" s="5" t="n">
         <v>12.07162</v>
       </c>
+      <c r="M27" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F28" s="1" t="n">
         <v>1987</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H28" s="1" t="n">
         <v>20</v>
@@ -2076,28 +2286,31 @@
       <c r="L28" s="5" t="n">
         <v>5.871512</v>
       </c>
+      <c r="M28" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F29" s="1" t="n">
         <v>2000</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>24</v>
@@ -2114,28 +2327,31 @@
       <c r="L29" s="5" t="n">
         <v>8.302932</v>
       </c>
+      <c r="M29" s="6" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F30" s="1" t="n">
         <v>2000</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H30" s="1" t="n">
         <v>20</v>
@@ -2152,28 +2368,31 @@
       <c r="L30" s="5" t="n">
         <v>6.550906</v>
       </c>
+      <c r="M30" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F31" s="1" t="n">
         <v>1985</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>24</v>
@@ -2190,28 +2409,31 @@
       <c r="L31" s="5" t="n">
         <v>4.770518</v>
       </c>
+      <c r="M31" s="6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F32" s="1" t="n">
         <v>1987</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H32" s="1" t="n">
         <v>19</v>
@@ -2228,28 +2450,31 @@
       <c r="L32" s="5" t="n">
         <v>7.049146</v>
       </c>
+      <c r="M32" s="6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F33" s="1" t="n">
         <v>1986</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H33" s="1" t="n">
         <v>22</v>
@@ -2266,28 +2491,31 @@
       <c r="L33" s="5" t="n">
         <v>12.43849</v>
       </c>
+      <c r="M33" s="6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F34" s="1" t="n">
         <v>1987</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H34" s="1" t="n">
         <v>8</v>
@@ -2304,28 +2532,31 @@
       <c r="L34" s="5" t="n">
         <v>3.258972</v>
       </c>
+      <c r="M34" s="6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H35" s="1" t="n">
         <v>20</v>
@@ -2342,28 +2573,31 @@
       <c r="L35" s="5" t="n">
         <v>2.571146</v>
       </c>
+      <c r="M35" s="6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F36" s="1" t="n">
         <v>1986</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H36" s="1" t="n">
         <v>9</v>
@@ -2380,28 +2614,31 @@
       <c r="L36" s="5" t="n">
         <v>5.658645</v>
       </c>
+      <c r="M36" s="6" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F37" s="1" t="n">
         <v>1988</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H37" s="1" t="n">
         <v>10</v>
@@ -2418,28 +2655,31 @@
       <c r="L37" s="5" t="n">
         <v>10.98257</v>
       </c>
+      <c r="M37" s="6" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F38" s="1" t="n">
         <v>1986</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H38" s="1" t="n">
         <v>24</v>
@@ -2456,28 +2696,31 @@
       <c r="L38" s="5" t="n">
         <v>6.84095</v>
       </c>
+      <c r="M38" s="6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F39" s="1" t="n">
         <v>1989</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H39" s="1" t="n">
         <v>11</v>
@@ -2494,28 +2737,31 @@
       <c r="L39" s="5" t="n">
         <v>9.276897</v>
       </c>
+      <c r="M39" s="6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F40" s="1" t="n">
         <v>1981</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H40" s="1" t="n">
         <v>24</v>
@@ -2532,28 +2778,31 @@
       <c r="L40" s="5" t="n">
         <v>5.254306</v>
       </c>
+      <c r="M40" s="6" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F41" s="1" t="n">
         <v>1988</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H41" s="1" t="n">
         <v>20</v>
@@ -2570,28 +2819,31 @@
       <c r="L41" s="5" t="n">
         <v>5.800668</v>
       </c>
+      <c r="M41" s="6" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F42" s="1" t="n">
         <v>1988</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H42" s="1" t="n">
         <v>24</v>
@@ -2608,28 +2860,31 @@
       <c r="L42" s="5" t="n">
         <v>7.509974</v>
       </c>
+      <c r="M42" s="6" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F43" s="1" t="n">
         <v>1987</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H43" s="1" t="n">
         <v>21</v>
@@ -2646,28 +2901,31 @@
       <c r="L43" s="5" t="n">
         <v>11.7434</v>
       </c>
+      <c r="M43" s="6" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F44" s="1" t="n">
         <v>1981</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H44" s="1" t="n">
         <v>12</v>
@@ -2684,28 +2942,31 @@
       <c r="L44" s="5" t="n">
         <v>2.58711</v>
       </c>
+      <c r="M44" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F45" s="1" t="n">
         <v>1986</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H45" s="1" t="n">
         <v>13</v>
@@ -2722,28 +2983,31 @@
       <c r="L45" s="5" t="n">
         <v>11.66763</v>
       </c>
+      <c r="M45" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F46" s="1" t="n">
         <v>1992</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H46" s="1" t="n">
         <v>14</v>
@@ -2760,28 +3024,31 @@
       <c r="L46" s="5" t="n">
         <v>8.550412</v>
       </c>
+      <c r="M46" s="6" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>154</v>
+        <v>181</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F47" s="1" t="n">
         <v>1987</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H47" s="1" t="n">
         <v>19</v>
@@ -2798,28 +3065,31 @@
       <c r="L47" s="5" t="n">
         <v>12.54876</v>
       </c>
+      <c r="M47" s="6" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F48" s="1" t="n">
         <v>1988</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H48" s="1" t="n">
         <v>24</v>
@@ -2836,28 +3106,31 @@
       <c r="L48" s="5" t="n">
         <v>7.561138</v>
       </c>
+      <c r="M48" s="6" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F49" s="1" t="n">
         <v>1989</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H49" s="1" t="n">
         <v>20</v>
@@ -2874,28 +3147,31 @@
       <c r="L49" s="5" t="n">
         <v>10.05889</v>
       </c>
+      <c r="M49" s="6" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F50" s="1" t="n">
         <v>1989</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H50" s="1" t="n">
         <v>19</v>
@@ -2912,28 +3188,31 @@
       <c r="L50" s="5" t="n">
         <v>2.909076</v>
       </c>
+      <c r="M50" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F51" s="1" t="n">
         <v>1983</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H51" s="1" t="n">
         <v>27</v>
@@ -2950,28 +3229,31 @@
       <c r="L51" s="5" t="n">
         <v>9.015336</v>
       </c>
+      <c r="M51" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F52" s="1" t="n">
         <v>1989</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H52" s="1" t="n">
         <v>24</v>
@@ -2988,28 +3270,31 @@
       <c r="L52" s="5" t="n">
         <v>3.467462</v>
       </c>
+      <c r="M52" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F53" s="1" t="n">
         <v>1981</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H53" s="1" t="n">
         <v>24</v>
@@ -3026,28 +3311,31 @@
       <c r="L53" s="5" t="n">
         <v>7.671867</v>
       </c>
+      <c r="M53" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F54" s="1" t="n">
         <v>1981</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H54" s="1" t="n">
         <v>15</v>
@@ -3064,28 +3352,31 @@
       <c r="L54" s="5" t="n">
         <v>6.927895</v>
       </c>
+      <c r="M54" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F55" s="1" t="n">
         <v>1988</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H55" s="1" t="n">
         <v>22</v>
@@ -3102,28 +3393,31 @@
       <c r="L55" s="5" t="n">
         <v>6.284053</v>
       </c>
+      <c r="M55" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F56" s="1" t="n">
         <v>1980</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H56" s="1" t="n">
         <v>16</v>
@@ -3140,28 +3434,31 @@
       <c r="L56" s="5" t="n">
         <v>5.823383</v>
       </c>
+      <c r="M56" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F57" s="1" t="n">
         <v>1994</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H57" s="1" t="n">
         <v>31</v>
@@ -3178,28 +3475,31 @@
       <c r="L57" s="5" t="n">
         <v>6.300305</v>
       </c>
+      <c r="M57" s="6" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F58" s="1" t="n">
         <v>1988</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H58" s="1" t="n">
         <v>17</v>
@@ -3216,28 +3516,31 @@
       <c r="L58" s="5" t="n">
         <v>2.925774</v>
       </c>
+      <c r="M58" s="6" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F59" s="1" t="n">
         <v>1989</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H59" s="1" t="n">
         <v>20</v>
@@ -3254,28 +3557,31 @@
       <c r="L59" s="5" t="n">
         <v>6.549802</v>
       </c>
+      <c r="M59" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>191</v>
+        <v>221</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>192</v>
+        <v>222</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>192</v>
+        <v>222</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>193</v>
+        <v>223</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F60" s="1" t="n">
         <v>1989</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H60" s="1" t="n">
         <v>18</v>
@@ -3292,28 +3598,31 @@
       <c r="L60" s="5" t="n">
         <v>12.21705</v>
       </c>
+      <c r="M60" s="6" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>195</v>
+        <v>226</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>195</v>
+        <v>226</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>196</v>
+        <v>227</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F61" s="1" t="n">
         <v>1989</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H61" s="1" t="n">
         <v>24</v>
@@ -3330,28 +3639,31 @@
       <c r="L61" s="5" t="n">
         <v>2.512377</v>
       </c>
+      <c r="M61" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>197</v>
+        <v>228</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>198</v>
+        <v>229</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>198</v>
+        <v>229</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>199</v>
+        <v>230</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F62" s="1" t="n">
         <v>1988</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H62" s="1" t="n">
         <v>19</v>
@@ -3368,28 +3680,31 @@
       <c r="L62" s="5" t="n">
         <v>7.51986</v>
       </c>
+      <c r="M62" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>200</v>
+        <v>231</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>201</v>
+        <v>232</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>201</v>
+        <v>232</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>202</v>
+        <v>233</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F63" s="1" t="n">
         <v>1988</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H63" s="1" t="n">
         <v>24</v>
@@ -3406,28 +3721,31 @@
       <c r="L63" s="5" t="n">
         <v>6.472228</v>
       </c>
+      <c r="M63" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>203</v>
+        <v>234</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>204</v>
+        <v>235</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>204</v>
+        <v>235</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>205</v>
+        <v>236</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F64" s="1" t="n">
         <v>1989</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H64" s="1" t="n">
         <v>30</v>
@@ -3444,28 +3762,31 @@
       <c r="L64" s="5" t="n">
         <v>7.729521</v>
       </c>
+      <c r="M64" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>206</v>
+        <v>237</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>207</v>
+        <v>238</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>207</v>
+        <v>238</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>209</v>
+        <v>240</v>
       </c>
       <c r="F65" s="1" t="n">
         <v>1980</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H65" s="1" t="n">
         <v>27</v>
@@ -3482,28 +3803,31 @@
       <c r="L65" s="5" t="n">
         <v>8.774425</v>
       </c>
+      <c r="M65" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>210</v>
+        <v>241</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>212</v>
+        <v>243</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F66" s="1" t="n">
         <v>1990</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H66" s="1" t="n">
         <v>20</v>
@@ -3520,28 +3844,31 @@
       <c r="L66" s="5" t="n">
         <v>7.172971</v>
       </c>
+      <c r="M66" s="6" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>213</v>
+        <v>245</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>215</v>
+        <v>247</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F67" s="1" t="n">
         <v>1988</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H67" s="1" t="n">
         <v>27</v>
@@ -3558,28 +3885,31 @@
       <c r="L67" s="5" t="n">
         <v>7.096405</v>
       </c>
+      <c r="M67" s="6" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>216</v>
+        <v>249</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>217</v>
+        <v>250</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>217</v>
+        <v>250</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F68" s="1" t="n">
         <v>1991</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H68" s="1" t="n">
         <v>27</v>
@@ -3596,28 +3926,31 @@
       <c r="L68" s="5" t="n">
         <v>5.671915</v>
       </c>
+      <c r="M68" s="6" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>219</v>
+        <v>253</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>220</v>
+        <v>254</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>220</v>
+        <v>254</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>221</v>
+        <v>255</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F69" s="1" t="n">
         <v>1980</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H69" s="1" t="n">
         <v>21</v>
@@ -3634,28 +3967,31 @@
       <c r="L69" s="5" t="n">
         <v>7.098576</v>
       </c>
+      <c r="M69" s="6" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>222</v>
+        <v>256</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>224</v>
+        <v>258</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>209</v>
+        <v>240</v>
       </c>
       <c r="F70" s="1" t="n">
         <v>1990</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H70" s="1" t="n">
         <v>22</v>
@@ -3672,28 +4008,31 @@
       <c r="L70" s="5" t="n">
         <v>9.265839</v>
       </c>
+      <c r="M70" s="6" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>225</v>
+        <v>260</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>227</v>
+        <v>262</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F71" s="1" t="n">
         <v>1990</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H71" s="1" t="n">
         <v>23</v>
@@ -3710,28 +4049,31 @@
       <c r="L71" s="5" t="n">
         <v>4.555897</v>
       </c>
+      <c r="M71" s="6" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>228</v>
+        <v>264</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>229</v>
+        <v>265</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>229</v>
+        <v>265</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F72" s="1" t="n">
         <v>1991</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H72" s="1" t="n">
         <v>24</v>
@@ -3748,28 +4090,31 @@
       <c r="L72" s="5" t="n">
         <v>9.53429</v>
       </c>
+      <c r="M72" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>231</v>
+        <v>267</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>233</v>
+        <v>269</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F73" s="1" t="n">
         <v>1990</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H73" s="1" t="n">
         <v>31</v>
@@ -3786,28 +4131,31 @@
       <c r="L73" s="5" t="n">
         <v>12.84202</v>
       </c>
+      <c r="M73" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>235</v>
+        <v>271</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>235</v>
+        <v>271</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F74" s="1" t="n">
         <v>1980</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H74" s="1" t="n">
         <v>25</v>
@@ -3824,28 +4172,31 @@
       <c r="L74" s="5" t="n">
         <v>9.158118</v>
       </c>
+      <c r="M74" s="6" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>237</v>
+        <v>273</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>238</v>
+        <v>274</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>238</v>
+        <v>274</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>239</v>
+        <v>275</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F75" s="1" t="n">
         <v>1980</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H75" s="1" t="n">
         <v>26</v>
@@ -3862,28 +4213,31 @@
       <c r="L75" s="5" t="n">
         <v>3.242612</v>
       </c>
+      <c r="M75" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>240</v>
+        <v>276</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>241</v>
+        <v>277</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>241</v>
+        <v>277</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>242</v>
+        <v>278</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F76" s="1" t="n">
         <v>1980</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H76" s="1" t="n">
         <v>27</v>
@@ -3900,28 +4254,31 @@
       <c r="L76" s="5" t="n">
         <v>3.325067</v>
       </c>
+      <c r="M76" s="6" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>243</v>
+        <v>279</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>244</v>
+        <v>280</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>244</v>
+        <v>280</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H77" s="1" t="n">
         <v>28</v>
@@ -3938,28 +4295,31 @@
       <c r="L77" s="5" t="n">
         <v>9.385772</v>
       </c>
+      <c r="M77" s="6" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>246</v>
+        <v>283</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>247</v>
+        <v>284</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>247</v>
+        <v>284</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>248</v>
+        <v>285</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H78" s="1" t="n">
         <v>29</v>
@@ -3976,28 +4336,31 @@
       <c r="L78" s="5" t="n">
         <v>2.546933</v>
       </c>
+      <c r="M78" s="6" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>249</v>
+        <v>287</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>250</v>
+        <v>288</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>250</v>
+        <v>288</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>251</v>
+        <v>289</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F79" s="1" t="n">
         <v>1994</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H79" s="1" t="n">
         <v>30</v>
@@ -4014,28 +4377,31 @@
       <c r="L79" s="5" t="n">
         <v>10.73155</v>
       </c>
+      <c r="M79" s="6" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>252</v>
+        <v>290</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>253</v>
+        <v>291</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>253</v>
+        <v>291</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>254</v>
+        <v>292</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F80" s="1" t="n">
         <v>1990</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H80" s="1" t="n">
         <v>31</v>
@@ -4052,28 +4418,31 @@
       <c r="L80" s="5" t="n">
         <v>2.816311</v>
       </c>
+      <c r="M80" s="6" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>255</v>
+        <v>293</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>256</v>
+        <v>294</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>256</v>
+        <v>294</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>257</v>
+        <v>295</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F81" s="1" t="n">
         <v>2004</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H81" s="1" t="n">
         <v>32</v>
@@ -4090,28 +4459,31 @@
       <c r="L81" s="5" t="n">
         <v>8.513116</v>
       </c>
+      <c r="M81" s="6" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>258</v>
+        <v>297</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>259</v>
+        <v>298</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>259</v>
+        <v>298</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>260</v>
+        <v>299</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F82" s="1" t="n">
         <v>1992</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H82" s="1" t="n">
         <v>32</v>
@@ -4127,12 +4499,15 @@
       </c>
       <c r="L82" s="5" t="n">
         <v>2.071624</v>
+      </c>
+      <c r="M82" s="7" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>